<commit_message>
Backlog do produto e backlog 3ª sprint
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog.xlsx
+++ b/Documentação/Backlog/Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Plant.ai\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Plant.ai\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
   <si>
     <t>Backlog do Projeto</t>
   </si>
@@ -340,6 +340,12 @@
   </si>
   <si>
     <t>3ªSprint</t>
+  </si>
+  <si>
+    <t>RP13</t>
+  </si>
+  <si>
+    <t>Ter uma Ferramenta Help Desk de suporte ao cliente</t>
   </si>
 </sst>
 </file>
@@ -349,7 +355,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,21 +406,48 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,8 +460,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -611,11 +650,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -624,15 +675,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -645,9 +687,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -669,34 +708,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,21 +722,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="40% - Ênfase6" xfId="1" builtinId="51"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -732,296 +800,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>902891</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1160860</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Multiplicar 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11439922" y="8483203"/>
-          <a:ext cx="257969" cy="257969"/>
-        </a:xfrm>
-        <a:prstGeom prst="mathMultiply">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>962422</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>138906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1220391</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>9922</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Multiplicar 2"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11499453" y="9217422"/>
-          <a:ext cx="257969" cy="257969"/>
-        </a:xfrm>
-        <a:prstGeom prst="mathMultiply">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>926307</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>281384</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1184276</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>53181</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Multiplicar 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11463338" y="10143728"/>
-          <a:ext cx="257969" cy="257969"/>
-        </a:xfrm>
-        <a:prstGeom prst="mathMultiply">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>926307</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1184276</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>53181</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Multiplicar 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11463338" y="10153650"/>
-          <a:ext cx="257969" cy="257969"/>
-        </a:xfrm>
-        <a:prstGeom prst="mathMultiply">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>926307</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>281384</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1184276</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Multiplicar 5"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11463338" y="13679884"/>
-          <a:ext cx="257969" cy="254000"/>
-        </a:xfrm>
-        <a:prstGeom prst="mathMultiply">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent2"/>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1287,895 +1065,936 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="106.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14" style="15" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14" style="11" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="11" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="23"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E4" s="17"/>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="E4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" s="32" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+    </row>
+    <row r="6" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>1192084</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="33" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+    </row>
+    <row r="7" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>1192099</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+    </row>
+    <row r="8" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <v>1192091</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="33" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+    </row>
+    <row r="9" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
         <v>1192027</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="13">
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
         <v>1192079</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="33" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:7" s="32" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
         <v>1192107</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="34" t="s">
         <v>94</v>
       </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="41" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="26">
+      <c r="C15" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="35">
         <v>5</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="26">
+      <c r="C16" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="35">
         <v>5</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="26">
+      <c r="C17" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="35">
         <v>3</v>
       </c>
-      <c r="F17" s="33" t="s">
+      <c r="F17" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="26" t="s">
+      <c r="G17" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="26">
+      <c r="C18" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="35">
         <v>3</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="26" t="s">
+      <c r="G18" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="26">
+      <c r="C19" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="35">
         <v>8</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="26" t="s">
+      <c r="G19" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
+    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="34">
+      <c r="C20" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="38">
         <v>21</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="26" t="s">
+      <c r="G20" s="35" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
+    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="26">
+      <c r="C21" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="35">
         <v>21</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="26" t="s">
+      <c r="G21" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="26">
+      <c r="C22" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="35">
         <v>21</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="26" t="s">
+      <c r="G22" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
+    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="26">
+      <c r="C23" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="35">
         <v>21</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="26">
+      <c r="C24" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="35">
         <v>3</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="26" t="s">
+      <c r="G24" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="26">
+      <c r="C25" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="35">
         <v>13</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G25" s="26" t="s">
+      <c r="G25" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
+    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="26">
+      <c r="C26" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="35">
         <v>21</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="26" t="s">
+      <c r="G26" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="32" t="s">
+    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A29" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B29" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32" t="s">
+      <c r="C29" s="41"/>
+      <c r="D29" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E29" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="32" t="s">
+      <c r="F29" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G29" s="41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
+    <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B30" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="26">
+      <c r="C30" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="35">
         <v>13</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F30" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G30" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+    <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B31" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C30" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="26" t="s">
+      <c r="C31" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="26">
+      <c r="E31" s="35">
         <v>5</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F31" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G30" s="26" t="s">
+      <c r="G31" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
+    <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B32" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C31" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="26" t="s">
+      <c r="C32" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="26">
+      <c r="E32" s="35">
         <v>5</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F32" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="26" t="s">
+      <c r="G32" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B33" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="26" t="s">
+      <c r="C33" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="26">
+      <c r="E33" s="35">
         <v>5</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F33" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G32" s="26" t="s">
+      <c r="G33" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="26" t="s">
+    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B34" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="26" t="s">
+      <c r="C34" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="26">
+      <c r="E34" s="35">
         <v>5</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F34" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="26" t="s">
+      <c r="G34" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="26" t="s">
+    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B35" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="26">
+      <c r="C35" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="35">
         <v>3</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="F35" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G35" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="26" t="s">
+    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B36" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C36" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D36" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="26">
+      <c r="E36" s="35">
         <v>3</v>
       </c>
-      <c r="F35" s="33" t="s">
+      <c r="F36" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G35" s="26" t="s">
+      <c r="G36" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B37" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="26">
+      <c r="C37" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="35">
         <v>21</v>
       </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26" t="s">
+      <c r="F37" s="35"/>
+      <c r="G37" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
+    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B38" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C38" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D37" s="26" t="s">
+      <c r="D38" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="26">
+      <c r="E38" s="35">
         <v>21</v>
       </c>
-      <c r="F37" s="26" t="s">
+      <c r="F38" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G37" s="26" t="s">
+      <c r="G38" s="35" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="26" t="s">
+    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="27" t="s">
+      <c r="B39" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C39" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="26">
+      <c r="D39" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="35">
         <v>13</v>
       </c>
-      <c r="F38" s="33" t="s">
+      <c r="F39" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G38" s="26" t="s">
+      <c r="G39" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="26" t="s">
+    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="B39" s="27" t="s">
+      <c r="B40" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C40" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="26">
+      <c r="D40" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="35">
         <v>8</v>
       </c>
-      <c r="F39" s="33" t="s">
+      <c r="F40" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G39" s="26" t="s">
+      <c r="G40" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="26" t="s">
+    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B41" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C41" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="26">
+      <c r="D41" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="35">
         <v>21</v>
       </c>
-      <c r="F40" s="33" t="s">
+      <c r="F41" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G40" s="26" t="s">
+      <c r="G41" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="26" t="s">
+    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B42" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="26">
+      <c r="C42" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="35">
         <v>21</v>
       </c>
-      <c r="F41" s="26" t="s">
+      <c r="F42" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G41" s="26" t="s">
+      <c r="G42" s="35" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="26"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="32" t="s">
+    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A44" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B44" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="32"/>
-      <c r="D43" s="32" t="s">
+      <c r="C44" s="41"/>
+      <c r="D44" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="32" t="s">
+      <c r="E44" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F43" s="32" t="s">
+      <c r="F44" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="G43" s="32" t="s">
+      <c r="G44" s="41" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B45" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D44" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E44" s="26">
+      <c r="C45" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="35">
         <v>8</v>
       </c>
-      <c r="F44" s="33" t="s">
+      <c r="F45" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G45" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B46" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="26">
+      <c r="C46" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="35">
         <v>13</v>
       </c>
-      <c r="F45" s="26" t="s">
+      <c r="F46" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="G45" s="26" t="s">
+      <c r="G46" s="35" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B47" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C46" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="28">
+      <c r="C47" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="44">
         <v>8</v>
       </c>
-      <c r="F46" s="33" t="s">
+      <c r="F47" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="G46" s="26" t="s">
+      <c r="G47" s="35" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-    </row>
-    <row r="55" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B55" s="19" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+    </row>
+    <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C55" s="19">
+      <c r="C56" s="15">
         <v>2</v>
       </c>
-      <c r="D55" s="18"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
+      <c r="D56" s="14"/>
+    </row>
+    <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B59" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D58" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E58" s="29">
+      <c r="C59" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="18">
         <v>21</v>
       </c>
-      <c r="F58" s="29" t="s">
+      <c r="F59" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G58" s="29" t="s">
+      <c r="G59" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="30" t="s">
+    <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B60" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="C59" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="31">
+      <c r="C60" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="20">
         <v>8</v>
       </c>
-      <c r="F59" s="29" t="s">
+      <c r="F60" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="G59" s="29" t="s">
+      <c r="G60" s="18" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2183,7 +2002,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2192,7 +2010,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,7 +2036,7 @@
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="12" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arquivo fluxograma formato drawn.io
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog.xlsx
+++ b/Documentação/Backlog/Backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\Plant.ai\Documentação\Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Plant.ai\Documentação\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="7035"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="7035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="105">
   <si>
     <t>Backlog do Projeto</t>
   </si>
@@ -666,7 +666,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -722,28 +722,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -783,6 +761,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1067,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A31" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1082,104 +1078,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:7" s="32" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:7" s="24" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>1192084</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-    </row>
-    <row r="7" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>1192099</v>
       </c>
-      <c r="B7" s="33" t="s">
+      <c r="B7" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-    </row>
-    <row r="8" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>1192091</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-    </row>
-    <row r="9" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>1192027</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-    </row>
-    <row r="10" spans="1:7" s="32" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+    </row>
+    <row r="10" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>1192079</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-    </row>
-    <row r="11" spans="1:7" s="32" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+    </row>
+    <row r="11" spans="1:7" s="24" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
         <v>1192107</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -1189,320 +1185,322 @@
       <c r="A13" s="7"/>
     </row>
     <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="41" t="s">
+      <c r="F14" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="35">
+      <c r="C15" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="27">
         <v>5</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="35">
+      <c r="C16" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="27">
         <v>5</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="35">
+      <c r="C17" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="27">
         <v>3</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="35">
+      <c r="C18" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="27">
         <v>3</v>
       </c>
-      <c r="F18" s="37" t="s">
+      <c r="F18" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="35">
+      <c r="C19" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="27">
         <v>8</v>
       </c>
-      <c r="F19" s="35" t="s">
+      <c r="F19" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="38">
+      <c r="C20" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="30">
         <v>21</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="35" t="s">
+      <c r="G20" s="27" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="35">
+      <c r="C21" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="27">
         <v>21</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="35">
+      <c r="C22" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="27">
         <v>21</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="35" t="s">
+      <c r="G22" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="35">
+      <c r="C23" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="27">
         <v>21</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="G23" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="35">
+      <c r="C24" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="27">
         <v>3</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="35" t="s">
+      <c r="G24" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="35">
+      <c r="C25" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="27">
         <v>13</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="G25" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="35">
+      <c r="C26" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="27">
         <v>21</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="35" t="s">
-        <v>89</v>
+      <c r="G26" s="27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="27"/>
+      <c r="D27" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="36"/>
       <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
+      <c r="G27" s="27" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
@@ -1514,320 +1512,320 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41" t="s">
+      <c r="C29" s="33"/>
+      <c r="D29" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="41" t="s">
+      <c r="E29" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="41" t="s">
+      <c r="F29" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="41" t="s">
+      <c r="G29" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="35">
+      <c r="C30" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="27">
         <v>13</v>
       </c>
-      <c r="F30" s="37" t="s">
+      <c r="F30" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="35" t="s">
+      <c r="C31" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E31" s="27">
         <v>5</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G31" s="35" t="s">
+      <c r="G31" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="35">
+      <c r="E32" s="27">
         <v>5</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="35" t="s">
+      <c r="C33" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E33" s="27">
         <v>5</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="35" t="s">
+      <c r="C34" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="35">
+      <c r="E34" s="27">
         <v>5</v>
       </c>
-      <c r="F34" s="37" t="s">
+      <c r="F34" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G34" s="35" t="s">
+      <c r="G34" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C35" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="35">
+      <c r="C35" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="27">
         <v>3</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F35" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G35" s="35" t="s">
+      <c r="G35" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="35">
+      <c r="E36" s="27">
         <v>3</v>
       </c>
-      <c r="F36" s="37" t="s">
+      <c r="F36" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="35">
+      <c r="C37" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="27">
         <v>21</v>
       </c>
-      <c r="F37" s="35"/>
-      <c r="G37" s="35" t="s">
+      <c r="F37" s="27"/>
+      <c r="G37" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="E38" s="35">
+      <c r="E38" s="27">
         <v>21</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="27" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="35">
+      <c r="D39" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="27">
         <v>13</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="F39" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G39" s="35" t="s">
+      <c r="G39" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D40" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="35">
+      <c r="D40" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="27">
         <v>8</v>
       </c>
-      <c r="F40" s="37" t="s">
+      <c r="F40" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="35">
+      <c r="D41" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="27">
         <v>21</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F41" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G41" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="A42" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C42" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="35">
+      <c r="C42" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="27">
         <v>21</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G42" s="27" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1841,92 +1839,92 @@
       <c r="G43" s="16"/>
     </row>
     <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="41" t="s">
+      <c r="C44" s="33"/>
+      <c r="D44" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="41" t="s">
+      <c r="E44" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="41" t="s">
+      <c r="F44" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="G44" s="41" t="s">
+      <c r="G44" s="33" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C45" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="35">
+      <c r="C45" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="27">
         <v>8</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="F45" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="G45" s="27" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="35" t="s">
+      <c r="A46" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="35">
+      <c r="C46" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="27">
         <v>13</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="G46" s="35" t="s">
+      <c r="G46" s="27" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="C47" s="35" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E47" s="44">
+      <c r="C47" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="36">
         <v>8</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="G47" s="35" t="s">
+      <c r="G47" s="27" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2009,7 +2007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualizando Backlog do Produto
</commit_message>
<xml_diff>
--- a/Documentação/Backlog/Backlog.xlsx
+++ b/Documentação/Backlog/Backlog.xlsx
@@ -1,23 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Plant.ai\Documentação\Backlog\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="7035" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19320" windowHeight="7035"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
   <si>
     <t>Backlog do Projeto</t>
   </si>
@@ -345,17 +340,83 @@
     <t>RP13</t>
   </si>
   <si>
-    <t>Ter uma Ferramenta Help Desk de suporte ao cliente</t>
+    <t>RS15</t>
+  </si>
+  <si>
+    <t>Cria Dashboard com gráficos dos dados coletados</t>
+  </si>
+  <si>
+    <t>RP14</t>
+  </si>
+  <si>
+    <t>Fazer Manual de Instalação</t>
+  </si>
+  <si>
+    <t>RP15</t>
+  </si>
+  <si>
+    <t>Planilha de Homologação</t>
+  </si>
+  <si>
+    <t>RB4</t>
+  </si>
+  <si>
+    <t>RB5</t>
+  </si>
+  <si>
+    <t>RP16</t>
+  </si>
+  <si>
+    <t>Fazer Fluxograma do Processo de Atendimento do Suporte</t>
+  </si>
+  <si>
+    <t>Ter uma Ferramenta Help Desk de Suporte ao Cliente</t>
+  </si>
+  <si>
+    <t>RP17</t>
+  </si>
+  <si>
+    <t>Teste integrado do Analytics</t>
+  </si>
+  <si>
+    <t>RP18</t>
+  </si>
+  <si>
+    <t>Teste Integrado da Solução de IoT</t>
+  </si>
+  <si>
+    <t>RB6</t>
+  </si>
+  <si>
+    <t>Fazer Modelagem Conceitual do Banco de Dados</t>
+  </si>
+  <si>
+    <t>Fazer Modelagem Lógica do Banco de Dados</t>
+  </si>
+  <si>
+    <t>Fazer Dicionário de Dados</t>
+  </si>
+  <si>
+    <t>Armazenar os dados capturados do Arduino no Banco de Dados</t>
+  </si>
+  <si>
+    <t>Fazer integração do Arduíno com o Banco de Dados no Azure</t>
+  </si>
+  <si>
+    <t>RB7</t>
+  </si>
+  <si>
+    <t>Ter todas as Tabelas criadas do Azure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,13 +461,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -664,9 +718,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -708,58 +762,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -779,6 +823,53 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -841,7 +932,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -876,7 +967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1053,976 +1144,1176 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="6" customWidth="1"/>
     <col min="2" max="2" width="106.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="11" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="11" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="4" spans="1:7" ht="24.95" customHeight="1" thickBot="1">
       <c r="E4" s="13"/>
     </row>
-    <row r="5" spans="1:7" s="24" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
+      <c r="A5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1">
       <c r="A6" s="8">
         <v>1192084</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-    </row>
-    <row r="7" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1">
       <c r="A7" s="9">
         <v>1192099</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="8" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+    </row>
+    <row r="8" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1">
       <c r="A8" s="9">
         <v>1192091</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-    </row>
-    <row r="9" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1">
       <c r="A9" s="9">
         <v>1192027</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-    </row>
-    <row r="10" spans="1:7" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1">
       <c r="A10" s="9">
         <v>1192079</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-    </row>
-    <row r="11" spans="1:7" s="24" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:7" s="20" customFormat="1" ht="24.95" customHeight="1" thickBot="1">
       <c r="A11" s="10">
         <v>1192107</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+    </row>
+    <row r="12" spans="1:7" ht="24.95" customHeight="1">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="24.95" customHeight="1">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+    <row r="14" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="33" t="s">
+      <c r="F14" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="33" t="s">
+      <c r="G14" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="27">
+      <c r="C15" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="23">
         <v>5</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A16" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="27">
+      <c r="C16" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="23">
         <v>5</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+    <row r="17" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A17" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="27">
+      <c r="C17" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="23">
         <v>3</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G17" s="27" t="s">
+      <c r="G17" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+    <row r="18" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A18" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="27">
+      <c r="C18" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="23">
         <v>3</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="27" t="s">
+      <c r="G18" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A19" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="27">
+      <c r="C19" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="23">
         <v>8</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="G19" s="27" t="s">
+      <c r="G19" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="20" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A20" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="30">
+      <c r="C20" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="26">
         <v>21</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="G20" s="27" t="s">
+      <c r="G20" s="23" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A21" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C21" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="27">
+      <c r="C21" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="23">
         <v>21</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A22" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="27">
+      <c r="C22" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="23">
         <v>21</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="G22" s="27" t="s">
+      <c r="G22" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A23" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="27">
+      <c r="C23" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="23">
         <v>21</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A24" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="27">
+      <c r="C24" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="23">
         <v>3</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="27" t="s">
+      <c r="G24" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="25" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A25" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" s="27">
+      <c r="C25" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="23">
         <v>13</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G25" s="27" t="s">
+      <c r="G25" s="23" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="26" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A26" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="27">
+      <c r="C26" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="23">
         <v>21</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="27" t="s">
+      <c r="G26" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+    <row r="27" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A27" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="32"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A28" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="32"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A29" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="32"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A30" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="B30" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="32"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A31" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="32"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A32" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="32"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A33" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="23"/>
+    </row>
+    <row r="34" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A34" s="15"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A35" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A36" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="23">
+        <v>13</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G36" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A37" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="23">
+        <v>5</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G37" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A38" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" s="23">
+        <v>5</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A39" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" s="23">
+        <v>5</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G39" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A40" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="23">
+        <v>5</v>
+      </c>
+      <c r="F40" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A41" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D41" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="23">
+        <v>3</v>
+      </c>
+      <c r="F41" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="23">
+        <v>3</v>
+      </c>
+      <c r="F42" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G42" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A43" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="23">
+        <v>21</v>
+      </c>
+      <c r="F43" s="23"/>
+      <c r="G43" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A44" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" s="23">
+        <v>21</v>
+      </c>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A45" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C45" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="23">
+        <v>13</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A46" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E46" s="23">
+        <v>8</v>
+      </c>
+      <c r="F46" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A47" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="23">
+        <v>21</v>
+      </c>
+      <c r="F47" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A48" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="23">
+        <v>21</v>
+      </c>
+      <c r="F48" s="23"/>
+      <c r="G48" s="23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A49" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="B49" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="36" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="27" t="s">
+      <c r="D49" s="41" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="41"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-    </row>
-    <row r="29" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="33" t="s">
+    <row r="50" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A50" s="15"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+    </row>
+    <row r="51" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A51" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33" t="s">
+      <c r="B51" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E51" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F51" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="33" t="s">
+      <c r="G51" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="27">
+    <row r="52" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A52" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="48">
+        <v>8</v>
+      </c>
+      <c r="F52" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G52" s="48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A53" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="48" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A54" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D54" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="48">
         <v>13</v>
       </c>
-      <c r="F30" s="29" t="s">
+      <c r="F54" s="48"/>
+      <c r="G54" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A55" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" s="50" t="s">
+        <v>123</v>
+      </c>
+      <c r="C55" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="51">
+        <v>8</v>
+      </c>
+      <c r="F55" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G55" s="48" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="27">
-        <v>5</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="27">
-        <v>5</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E33" s="27">
-        <v>5</v>
-      </c>
-      <c r="F33" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G33" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E34" s="27">
-        <v>5</v>
-      </c>
-      <c r="F34" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G34" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="27">
-        <v>3</v>
-      </c>
-      <c r="F35" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G35" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="27" t="s">
+    <row r="56" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A56" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C56" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="51"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A57" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="B57" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="53"/>
+      <c r="F57" s="53"/>
+      <c r="G57" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A58" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="B58" s="50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C58" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="D36" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" s="27">
-        <v>3</v>
-      </c>
-      <c r="F36" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G36" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="D58" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="55"/>
+      <c r="F58" s="53"/>
+      <c r="G58" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A66" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="30">
+        <v>2</v>
+      </c>
+      <c r="D66" s="14"/>
+    </row>
+    <row r="67" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A67" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B67" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="27">
+      <c r="C67" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D67" s="43" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="43">
         <v>21</v>
       </c>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="27">
-        <v>21</v>
-      </c>
-      <c r="F38" s="27" t="s">
+      <c r="F67" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="G38" s="27" t="s">
+      <c r="G67" s="43" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="27">
-        <v>13</v>
-      </c>
-      <c r="F39" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G39" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="27">
+    <row r="68" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A68" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="45">
         <v>8</v>
       </c>
-      <c r="F40" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="B41" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="27">
-        <v>21</v>
-      </c>
-      <c r="F41" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G41" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="27">
-        <v>21</v>
-      </c>
-      <c r="F42" s="27" t="s">
+      <c r="F68" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="27" t="s">
+      <c r="G68" s="43" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-    </row>
-    <row r="44" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" s="33"/>
-      <c r="D44" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="F44" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" s="27">
-        <v>8</v>
-      </c>
-      <c r="F45" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G45" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E46" s="27">
-        <v>13</v>
-      </c>
-      <c r="F46" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="G46" s="27" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E47" s="36">
-        <v>8</v>
-      </c>
-      <c r="F47" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="G47" s="27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-    </row>
-    <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C56" s="15">
-        <v>2</v>
-      </c>
-      <c r="D56" s="14"/>
-    </row>
-    <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D59" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E59" s="18">
-        <v>21</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G59" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C60" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D60" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="20">
-        <v>8</v>
-      </c>
-      <c r="F60" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="G60" s="18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
+    <row r="69" spans="1:7" ht="24.95" customHeight="1">
+      <c r="A69" s="27"/>
+      <c r="B69" s="40"/>
+      <c r="C69" s="46"/>
+      <c r="D69" s="46"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="40"/>
+      <c r="G69" s="40"/>
+    </row>
+    <row r="70" spans="1:7" ht="24.95" customHeight="1">
+      <c r="B70" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="44" fitToWidth="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="94.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -2030,7 +2321,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="26.25">
       <c r="A3" s="1" t="s">
         <v>63</v>
       </c>
@@ -2038,136 +2329,136 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="15.75" thickBot="1">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="15.75" thickBot="1">
       <c r="A29" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1">
       <c r="A30" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1">
       <c r="A31" s="1" t="s">
         <v>59</v>
       </c>

</xml_diff>